<commit_message>
Update string lastAssignedBy to be null
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D0FA0-295D-4293-B774-80DC28EFF37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38281259-E68A-4B17-B765-93376F2E9AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9662" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9673" uniqueCount="865">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5431,7 +5431,7 @@
     <t>Ghi Chú 1</t>
   </si>
   <si>
-    <t>197pm21905</t>
+    <t>hehe</t>
   </si>
 </sst>
 </file>
@@ -6352,10 +6352,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y4" sqref="Y4"/>
+      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6646,8 +6646,8 @@
       <c r="X3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="Y3" s="8">
-        <v>4</v>
+      <c r="Y3" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>51</v>
@@ -6907,7 +6907,9 @@
       <c r="O6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="12"/>
+      <c r="P6" s="12" t="s">
+        <v>864</v>
+      </c>
       <c r="Q6" s="12" t="s">
         <v>43</v>
       </c>
@@ -8727,8 +8729,8 @@
       <c r="O25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="P25" s="8">
-        <v>2001102245</v>
+      <c r="P25" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>123</v>
@@ -9399,8 +9401,8 @@
       <c r="O32" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="P32" s="10">
-        <v>2001102245</v>
+      <c r="P32" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="Q32" s="10" t="s">
         <v>140</v>
@@ -9498,7 +9500,7 @@
         <v>167</v>
       </c>
       <c r="P33" s="11" t="s">
-        <v>864</v>
+        <v>38</v>
       </c>
       <c r="Q33" s="11" t="s">
         <v>75</v>
@@ -10954,8 +10956,8 @@
       <c r="X48" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="Y48" s="8">
-        <v>0</v>
+      <c r="Y48" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="Z48" s="8" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Update alert to guide user to import lecturer
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38281259-E68A-4B17-B765-93376F2E9AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96356DB0-C1C4-47D0-BF1B-5B5E0D050612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9673" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9666" uniqueCount="865">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6355,7 +6355,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6524,7 +6524,7 @@
         <v>42</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>38</v>
+        <v>864</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>43</v>
@@ -6907,9 +6907,7 @@
       <c r="O6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="P6" s="12" t="s">
-        <v>864</v>
-      </c>
+      <c r="P6" s="12"/>
       <c r="Q6" s="12" t="s">
         <v>43</v>
       </c>

</xml_diff>